<commit_message>
Finished and turned in project
</commit_message>
<xml_diff>
--- a/Project/Manual checks.xlsx
+++ b/Project/Manual checks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mick\Documents\Class\ME599 - Python\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D7CA49F-E24C-4C3B-93E5-982CD4226999}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D542454-6F6A-405E-9F2E-CD99AF619904}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1" xr2:uid="{961913D4-C432-44FC-8894-294E91817694}"/>
   </bookViews>
@@ -153,8 +153,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="0.0000"/>
-    <numFmt numFmtId="174" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -407,13 +407,85 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -425,11 +497,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -437,94 +506,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -871,28 +871,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="Q1" s="22" t="s">
+      <c r="Q1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
+      <c r="R1" s="49"/>
+      <c r="S1" s="49"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="18"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="52"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="1" t="s">
@@ -906,25 +906,25 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="16">
-        <v>1</v>
-      </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="16">
-        <v>0.75</v>
-      </c>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="18"/>
+      <c r="C3" s="50">
+        <v>1</v>
+      </c>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="50">
+        <v>0.75</v>
+      </c>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="52"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="1" t="s">
@@ -938,7 +938,7 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="23" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="15" t="s">
@@ -953,10 +953,10 @@
       <c r="F4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="36" t="s">
+      <c r="H4" s="25" t="s">
         <v>18</v>
       </c>
       <c r="I4" s="15" t="s">
@@ -971,13 +971,13 @@
       <c r="L4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="23" t="s">
+      <c r="M4" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="N4" s="36" t="s">
+      <c r="N4" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="P4" s="23"/>
+      <c r="P4" s="16"/>
       <c r="Q4" s="1" t="s">
         <v>0</v>
       </c>
@@ -989,20 +989,20 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="53">
-        <v>1</v>
-      </c>
-      <c r="D5" s="41">
+      <c r="C5" s="40">
+        <v>1</v>
+      </c>
+      <c r="D5" s="28">
         <f>$C5/SUM($C$5:$C$6)</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="E5" s="39">
+      <c r="E5" s="46">
         <f>C5/C6</f>
         <v>2</v>
       </c>
@@ -1014,18 +1014,18 @@
         <f>F5</f>
         <v>67550</v>
       </c>
-      <c r="H5" s="47">
+      <c r="H5" s="34">
         <f>S10*$R$2</f>
         <v>5.7218998680734151E-3</v>
       </c>
-      <c r="I5" s="53">
+      <c r="I5" s="40">
         <v>1</v>
       </c>
       <c r="J5" s="7">
         <f>$I5/SUM($I$5:$I$6)</f>
         <v>0.60000000000000009</v>
       </c>
-      <c r="K5" s="39">
+      <c r="K5" s="46">
         <f>I3*E5</f>
         <v>1.5</v>
       </c>
@@ -1037,13 +1037,13 @@
         <f>L5</f>
         <v>60795.000000000007</v>
       </c>
-      <c r="N5" s="47">
+      <c r="N5" s="34">
         <f>T10*$R$2</f>
         <v>5.1497098812660737E-3</v>
       </c>
-      <c r="O5" s="25"/>
-      <c r="P5" s="25"/>
-      <c r="Q5" s="23" t="s">
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="16" t="s">
         <v>22</v>
       </c>
       <c r="R5" s="1">
@@ -1054,18 +1054,18 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
-      <c r="B6" s="35" t="s">
+      <c r="A6" s="45"/>
+      <c r="B6" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="54">
+      <c r="C6" s="41">
         <v>0.5</v>
       </c>
-      <c r="D6" s="43">
+      <c r="D6" s="30">
         <f>$C6/SUM($C$5:$C$6)</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="E6" s="38"/>
+      <c r="E6" s="47"/>
       <c r="F6" s="4">
         <f>$R$4*D6</f>
         <v>33775</v>
@@ -1074,11 +1074,11 @@
         <f>F6+G5</f>
         <v>101325</v>
       </c>
-      <c r="H6" s="48">
+      <c r="H6" s="35">
         <f>S11*$R$2</f>
         <v>4.5412903917521771E-2</v>
       </c>
-      <c r="I6" s="54">
+      <c r="I6" s="41">
         <f>I5/K5</f>
         <v>0.66666666666666663</v>
       </c>
@@ -1086,7 +1086,7 @@
         <f>$I6/SUM($I$5:$I$6)</f>
         <v>0.4</v>
       </c>
-      <c r="K6" s="38"/>
+      <c r="K6" s="47"/>
       <c r="L6" s="4">
         <f>$R$4*J6</f>
         <v>40530</v>
@@ -1095,12 +1095,12 @@
         <f>L6+M5</f>
         <v>101325</v>
       </c>
-      <c r="N6" s="48">
+      <c r="N6" s="35">
         <f>T11*$R$2</f>
         <v>5.449548470102613E-2</v>
       </c>
-      <c r="O6" s="25"/>
-      <c r="P6" s="25"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
       <c r="Q6" s="1" t="s">
         <v>13</v>
       </c>
@@ -1109,20 +1109,20 @@
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="23" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="42">
+      <c r="D7" s="29">
         <f>D5</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="48">
         <f>E5</f>
         <v>2</v>
       </c>
@@ -1132,7 +1132,7 @@
       <c r="G7" s="3">
         <v>67550</v>
       </c>
-      <c r="H7" s="49">
+      <c r="H7" s="36">
         <v>5.7218998680700003E-3</v>
       </c>
       <c r="I7" s="15" t="s">
@@ -1142,42 +1142,42 @@
         <f>J5</f>
         <v>0.60000000000000009</v>
       </c>
-      <c r="K7" s="27">
+      <c r="K7" s="48">
         <f>K5</f>
         <v>1.5</v>
       </c>
-      <c r="L7" s="25">
+      <c r="L7" s="18">
         <v>60795.000000000007</v>
       </c>
       <c r="M7" s="3">
         <v>60795</v>
       </c>
-      <c r="N7" s="49">
+      <c r="N7" s="36">
         <v>5.1497098812700003E-3</v>
       </c>
-      <c r="O7" s="25"/>
-      <c r="P7" s="25"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="18"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
-      <c r="B8" s="35" t="s">
+      <c r="A8" s="45"/>
+      <c r="B8" s="24" t="s">
         <v>29</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="43">
+      <c r="D8" s="30">
         <f>D6</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="E8" s="38"/>
+      <c r="E8" s="47"/>
       <c r="F8" s="4">
         <v>33775</v>
       </c>
       <c r="G8" s="4">
         <v>101325</v>
       </c>
-      <c r="H8" s="50">
+      <c r="H8" s="37">
         <v>4.5412903917499997E-2</v>
       </c>
       <c r="I8" s="14" t="s">
@@ -1187,18 +1187,18 @@
         <f>J6</f>
         <v>0.4</v>
       </c>
-      <c r="K8" s="38"/>
-      <c r="L8" s="24">
+      <c r="K8" s="47"/>
+      <c r="L8" s="17">
         <v>40530</v>
       </c>
       <c r="M8" s="4">
         <v>101325</v>
       </c>
-      <c r="N8" s="50">
+      <c r="N8" s="37">
         <v>5.4495484700999998E-2</v>
       </c>
-      <c r="O8" s="25"/>
-      <c r="P8" s="25"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="18"/>
       <c r="S8" s="1">
         <v>1</v>
       </c>
@@ -1231,21 +1231,21 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="28"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="54"/>
+      <c r="M11" s="54"/>
+      <c r="N11" s="55"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="1" t="s">
@@ -1267,22 +1267,22 @@
       <c r="B12" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="16">
-        <v>1</v>
-      </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="16">
-        <v>0.75</v>
-      </c>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="18"/>
+      <c r="C12" s="50">
+        <v>1</v>
+      </c>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="50">
+        <v>0.75</v>
+      </c>
+      <c r="J12" s="51"/>
+      <c r="K12" s="51"/>
+      <c r="L12" s="51"/>
+      <c r="M12" s="51"/>
+      <c r="N12" s="52"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
     </row>
@@ -1302,10 +1302,10 @@
       <c r="F13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="23" t="s">
+      <c r="G13" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="40" t="s">
+      <c r="H13" s="27" t="s">
         <v>18</v>
       </c>
       <c r="I13" s="10" t="s">
@@ -1320,10 +1320,10 @@
       <c r="L13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="M13" s="23" t="s">
+      <c r="M13" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="N13" s="40" t="s">
+      <c r="N13" s="27" t="s">
         <v>18</v>
       </c>
       <c r="O13" s="3"/>
@@ -1336,20 +1336,20 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="43" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="53">
-        <v>1</v>
-      </c>
-      <c r="D14" s="44">
+      <c r="C14" s="40">
+        <v>1</v>
+      </c>
+      <c r="D14" s="31">
         <f>(1-D16)*C14/SUM(C14:C15)</f>
         <v>0.53333333333333333</v>
       </c>
-      <c r="E14" s="39">
+      <c r="E14" s="46">
         <f>D14/D15</f>
         <v>2</v>
       </c>
@@ -1365,14 +1365,14 @@
         <f>S14*$R$2</f>
         <v>4.5775198944587314E-3</v>
       </c>
-      <c r="I14" s="53">
+      <c r="I14" s="40">
         <v>1</v>
       </c>
       <c r="J14" s="7">
         <f>(1-J16)*I14/SUM(I14:I15)</f>
         <v>0.48000000000000009</v>
       </c>
-      <c r="K14" s="39">
+      <c r="K14" s="46">
         <f>I12*E14</f>
         <v>1.5</v>
       </c>
@@ -1384,12 +1384,12 @@
         <f>L14</f>
         <v>48636.000000000007</v>
       </c>
-      <c r="N14" s="47">
+      <c r="N14" s="34">
         <f>T14*$R$2</f>
         <v>4.1197679050128588E-3</v>
       </c>
-      <c r="O14" s="25"/>
-      <c r="P14" s="25"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="18"/>
       <c r="Q14" s="1" t="s">
         <v>4</v>
       </c>
@@ -1406,18 +1406,18 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
+      <c r="A15" s="44"/>
       <c r="B15" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="55">
+      <c r="C15" s="42">
         <v>0.5</v>
       </c>
-      <c r="D15" s="45">
+      <c r="D15" s="32">
         <f>(1-D16)*C15/SUM(C14:C15)</f>
         <v>0.26666666666666666</v>
       </c>
-      <c r="E15" s="27"/>
+      <c r="E15" s="48"/>
       <c r="F15" s="3">
         <f>$R$4*D15</f>
         <v>27020</v>
@@ -1430,7 +1430,7 @@
         <f>S15*$R$2</f>
         <v>3.633032313401742E-2</v>
       </c>
-      <c r="I15" s="55">
+      <c r="I15" s="42">
         <f>I14/K14</f>
         <v>0.66666666666666663</v>
       </c>
@@ -1438,7 +1438,7 @@
         <f>(1-J16)*I15/SUM(I14:I15)</f>
         <v>0.32</v>
       </c>
-      <c r="K15" s="27"/>
+      <c r="K15" s="48"/>
       <c r="L15" s="3">
         <f>$R$4*J15</f>
         <v>32424</v>
@@ -1447,12 +1447,12 @@
         <f>L15+M14</f>
         <v>81060</v>
       </c>
-      <c r="N15" s="51">
+      <c r="N15" s="38">
         <f>T15*$R$2</f>
         <v>4.35963877608209E-2</v>
       </c>
-      <c r="O15" s="25"/>
-      <c r="P15" s="25"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="18"/>
       <c r="Q15" s="1" t="s">
         <v>5</v>
       </c>
@@ -1469,19 +1469,19 @@
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
+      <c r="A16" s="45"/>
       <c r="B16" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="54">
+      <c r="C16" s="41">
         <f>R6*SUM(C14:C15)</f>
         <v>0.30000000000000004</v>
       </c>
-      <c r="D16" s="46">
+      <c r="D16" s="33">
         <f>R6</f>
         <v>0.2</v>
       </c>
-      <c r="E16" s="38"/>
+      <c r="E16" s="47"/>
       <c r="F16" s="4">
         <f>$R$4*D16</f>
         <v>20265</v>
@@ -1494,7 +1494,7 @@
         <f>S16*$R$2</f>
         <v>3.4016675982171077E-2</v>
       </c>
-      <c r="I16" s="54">
+      <c r="I16" s="41">
         <f>J16*SUM(I14:I15)</f>
         <v>0.33333333333333331</v>
       </c>
@@ -1502,7 +1502,7 @@
         <f>R6</f>
         <v>0.2</v>
       </c>
-      <c r="K16" s="38"/>
+      <c r="K16" s="47"/>
       <c r="L16" s="4">
         <f>$R$4*J16</f>
         <v>20265</v>
@@ -1511,16 +1511,16 @@
         <f>L16+M15</f>
         <v>101325</v>
       </c>
-      <c r="N16" s="48">
-        <f t="shared" ref="N15:N16" si="0">T16*$R$2</f>
+      <c r="N16" s="35">
+        <f t="shared" ref="N16" si="0">T16*$R$2</f>
         <v>3.4016675982171077E-2</v>
       </c>
-      <c r="O16" s="25"/>
-      <c r="P16" s="25"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="18"/>
       <c r="Q16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="R16" s="29">
+      <c r="R16" s="19">
         <v>39.948</v>
       </c>
       <c r="S16" s="1">
@@ -1528,12 +1528,12 @@
         <v>0.33090151733629453</v>
       </c>
       <c r="T16" s="1">
-        <f t="shared" ref="T15:T17" si="1">L16/($R$5*$R$3/R16)</f>
+        <f t="shared" ref="T16" si="1">L16/($R$5*$R$3/R16)</f>
         <v>0.33090151733629453</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="44" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="13" t="s">
@@ -1542,21 +1542,21 @@
       <c r="C17" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="45">
+      <c r="D17" s="32">
         <f>D14</f>
         <v>0.53333333333333333</v>
       </c>
-      <c r="E17" s="27">
+      <c r="E17" s="48">
         <f>E14</f>
         <v>2</v>
       </c>
-      <c r="F17" s="25">
+      <c r="F17" s="18">
         <v>54040</v>
       </c>
       <c r="G17" s="3">
         <v>54040</v>
       </c>
-      <c r="H17" s="37">
+      <c r="H17" s="26">
         <v>4.5775198944600004E-3</v>
       </c>
       <c r="I17" s="15" t="s">
@@ -1566,41 +1566,41 @@
         <f>J14</f>
         <v>0.48000000000000009</v>
       </c>
-      <c r="K17" s="27">
+      <c r="K17" s="48">
         <f>K14</f>
         <v>1.5</v>
       </c>
-      <c r="L17" s="25">
+      <c r="L17" s="18">
         <v>48636.000000000007</v>
       </c>
       <c r="M17" s="3">
         <v>48636</v>
       </c>
-      <c r="N17" s="52">
+      <c r="N17" s="39">
         <v>4.11976790501E-3</v>
       </c>
-      <c r="P17" s="25"/>
+      <c r="P17" s="18"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
+      <c r="A18" s="44"/>
       <c r="B18" s="15" t="s">
         <v>29</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="45">
+      <c r="D18" s="32">
         <f>D15</f>
         <v>0.26666666666666666</v>
       </c>
-      <c r="E18" s="27"/>
-      <c r="F18" s="25">
+      <c r="E18" s="48"/>
+      <c r="F18" s="18">
         <v>27020</v>
       </c>
       <c r="G18" s="3">
         <v>81060</v>
       </c>
-      <c r="H18" s="37">
+      <c r="H18" s="26">
         <v>3.63303231341E-2</v>
       </c>
       <c r="I18" s="15" t="s">
@@ -1610,32 +1610,32 @@
         <f>J15</f>
         <v>0.32</v>
       </c>
-      <c r="K18" s="27"/>
-      <c r="L18" s="25">
+      <c r="K18" s="48"/>
+      <c r="L18" s="18">
         <v>32424</v>
       </c>
       <c r="M18" s="3">
         <v>81060</v>
       </c>
-      <c r="N18" s="52">
+      <c r="N18" s="39">
         <v>4.35963877608E-2</v>
       </c>
-      <c r="P18" s="25"/>
+      <c r="P18" s="18"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
+      <c r="A19" s="45"/>
       <c r="B19" s="14" t="s">
         <v>30</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="46">
+      <c r="D19" s="33">
         <f>D16</f>
         <v>0.2</v>
       </c>
-      <c r="E19" s="38"/>
-      <c r="F19" s="24">
+      <c r="E19" s="47"/>
+      <c r="F19" s="17">
         <v>20265</v>
       </c>
       <c r="G19" s="4">
@@ -1651,17 +1651,17 @@
         <f>J16</f>
         <v>0.2</v>
       </c>
-      <c r="K19" s="38"/>
-      <c r="L19" s="24">
+      <c r="K19" s="47"/>
+      <c r="L19" s="17">
         <v>20265</v>
       </c>
       <c r="M19" s="4">
         <v>101325</v>
       </c>
-      <c r="N19" s="50">
+      <c r="N19" s="37">
         <v>3.4016675982199998E-2</v>
       </c>
-      <c r="P19" s="25"/>
+      <c r="P19" s="18"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F21"/>
@@ -1695,17 +1695,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="I3:N3"/>
-    <mergeCell ref="C12:H12"/>
-    <mergeCell ref="E14:E16"/>
     <mergeCell ref="K17:K19"/>
     <mergeCell ref="E17:E19"/>
     <mergeCell ref="K5:K6"/>
@@ -1713,7 +1702,18 @@
     <mergeCell ref="K14:K16"/>
     <mergeCell ref="I12:N12"/>
     <mergeCell ref="B11:N11"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="I3:N3"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="E14:E16"/>
     <mergeCell ref="B2:N2"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E7:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1723,8 +1723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3357807-3B09-48BD-A8EA-B412AFD2029C}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection sqref="A1:I32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1741,25 +1741,25 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="16" t="s">
+      <c r="C1" s="52"/>
+      <c r="D1" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="16" t="s">
+      <c r="E1" s="52"/>
+      <c r="F1" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="17" t="s">
+      <c r="G1" s="52"/>
+      <c r="H1" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="18"/>
+      <c r="I1" s="52"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="22" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="10" t="s">
@@ -1788,65 +1788,65 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="43" t="s">
         <v>36</v>
       </c>
       <c r="B3" s="13">
-        <v>1.25</v>
-      </c>
-      <c r="C3" s="30">
+        <v>0.75</v>
+      </c>
+      <c r="C3" s="20">
         <v>0</v>
       </c>
       <c r="D3" s="13">
-        <v>0.75</v>
-      </c>
-      <c r="E3" s="30">
+        <v>1</v>
+      </c>
+      <c r="E3" s="20">
         <v>0</v>
       </c>
       <c r="F3" s="13">
         <v>1</v>
       </c>
-      <c r="G3" s="30">
+      <c r="G3" s="20">
         <v>0</v>
       </c>
       <c r="H3" s="7">
-        <v>0.75</v>
-      </c>
-      <c r="I3" s="30">
+        <v>1.25</v>
+      </c>
+      <c r="I3" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
+      <c r="A4" s="44"/>
       <c r="B4" s="15">
         <v>1</v>
       </c>
-      <c r="C4" s="37">
+      <c r="C4" s="26">
         <v>0</v>
       </c>
       <c r="D4" s="15">
-        <v>1</v>
-      </c>
-      <c r="E4" s="37">
+        <v>0.75</v>
+      </c>
+      <c r="E4" s="26">
         <v>0</v>
       </c>
       <c r="F4" s="15">
         <v>0.75</v>
       </c>
-      <c r="G4" s="37">
+      <c r="G4" s="26">
         <v>0</v>
       </c>
       <c r="H4" s="3">
-        <v>1.25</v>
-      </c>
-      <c r="I4" s="37">
+        <v>0.75</v>
+      </c>
+      <c r="I4" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
+      <c r="A5" s="45"/>
       <c r="B5" s="14">
-        <v>0.75</v>
+        <v>1.25</v>
       </c>
       <c r="C5" s="12">
         <v>0</v>
@@ -1871,225 +1871,225 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="43" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="13">
-        <v>1.25</v>
-      </c>
-      <c r="C6" s="30">
+        <v>1</v>
+      </c>
+      <c r="C6" s="20">
         <v>0.3</v>
       </c>
       <c r="D6" s="13">
-        <v>1</v>
-      </c>
-      <c r="E6" s="30">
-        <v>0.1</v>
+        <v>0.75</v>
+      </c>
+      <c r="E6" s="20">
+        <v>0.2</v>
       </c>
       <c r="F6" s="13">
         <v>1.25</v>
       </c>
-      <c r="G6" s="30">
-        <v>0.2</v>
+      <c r="G6" s="20">
+        <v>0.3</v>
       </c>
       <c r="H6" s="7">
-        <v>1</v>
-      </c>
-      <c r="I6" s="30">
-        <v>0.1</v>
+        <v>1.25</v>
+      </c>
+      <c r="I6" s="20">
+        <v>0.2</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="15">
         <v>1</v>
       </c>
-      <c r="C7" s="37">
-        <v>0.2</v>
+      <c r="C7" s="26">
+        <v>0.1</v>
       </c>
       <c r="D7" s="15">
         <v>1.25</v>
       </c>
-      <c r="E7" s="37">
+      <c r="E7" s="26">
         <v>0.2</v>
       </c>
       <c r="F7" s="15">
         <v>1</v>
       </c>
-      <c r="G7" s="37">
+      <c r="G7" s="26">
         <v>0.3</v>
       </c>
       <c r="H7" s="3">
-        <v>1.25</v>
-      </c>
-      <c r="I7" s="37">
-        <v>0.3</v>
+        <v>1</v>
+      </c>
+      <c r="I7" s="26">
+        <v>0.1</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
+      <c r="A8" s="44"/>
       <c r="B8" s="15">
         <v>1</v>
       </c>
-      <c r="C8" s="37">
-        <v>0.1</v>
+      <c r="C8" s="26">
+        <v>0.2</v>
       </c>
       <c r="D8" s="15">
-        <v>0.75</v>
-      </c>
-      <c r="E8" s="37">
-        <v>0.3</v>
+        <v>1</v>
+      </c>
+      <c r="E8" s="26">
+        <v>0.1</v>
       </c>
       <c r="F8" s="15">
         <v>1</v>
       </c>
-      <c r="G8" s="37">
-        <v>0.1</v>
+      <c r="G8" s="26">
+        <v>0.2</v>
       </c>
       <c r="H8" s="3">
-        <v>1</v>
-      </c>
-      <c r="I8" s="37">
-        <v>0.3</v>
+        <v>1.25</v>
+      </c>
+      <c r="I8" s="26">
+        <v>0.1</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
+      <c r="A9" s="44"/>
       <c r="B9" s="15">
-        <v>0.75</v>
-      </c>
-      <c r="C9" s="37">
+        <v>1.25</v>
+      </c>
+      <c r="C9" s="26">
         <v>0.3</v>
       </c>
       <c r="D9" s="15">
-        <v>1.25</v>
-      </c>
-      <c r="E9" s="37">
+        <v>0.75</v>
+      </c>
+      <c r="E9" s="26">
         <v>0.1</v>
       </c>
       <c r="F9" s="15">
         <v>1.25</v>
       </c>
-      <c r="G9" s="37">
+      <c r="G9" s="26">
         <v>0.1</v>
       </c>
       <c r="H9" s="3">
-        <v>0.75</v>
-      </c>
-      <c r="I9" s="37">
-        <v>0.1</v>
+        <v>1.25</v>
+      </c>
+      <c r="I9" s="26">
+        <v>0.3</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
+      <c r="A10" s="44"/>
       <c r="B10" s="15">
-        <v>1</v>
-      </c>
-      <c r="C10" s="37">
-        <v>0.3</v>
+        <v>0.75</v>
+      </c>
+      <c r="C10" s="26">
+        <v>0.2</v>
       </c>
       <c r="D10" s="15">
-        <v>1.25</v>
-      </c>
-      <c r="E10" s="37">
+        <v>1</v>
+      </c>
+      <c r="E10" s="26">
         <v>0.3</v>
       </c>
       <c r="F10" s="15">
-        <v>0.75</v>
-      </c>
-      <c r="G10" s="37">
+        <v>1.25</v>
+      </c>
+      <c r="G10" s="26">
         <v>0.2</v>
       </c>
       <c r="H10" s="3">
-        <v>0.75</v>
-      </c>
-      <c r="I10" s="37">
-        <v>0.3</v>
+        <v>1</v>
+      </c>
+      <c r="I10" s="26">
+        <v>0.2</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
+      <c r="A11" s="44"/>
       <c r="B11" s="15">
-        <v>1.25</v>
-      </c>
-      <c r="C11" s="37">
-        <v>0.1</v>
+        <v>0.75</v>
+      </c>
+      <c r="C11" s="26">
+        <v>0.3</v>
       </c>
       <c r="D11" s="15">
-        <v>1</v>
-      </c>
-      <c r="E11" s="37">
+        <v>0.75</v>
+      </c>
+      <c r="E11" s="26">
         <v>0.3</v>
       </c>
       <c r="F11" s="15">
         <v>0.75</v>
       </c>
-      <c r="G11" s="37">
+      <c r="G11" s="26">
         <v>0.3</v>
       </c>
       <c r="H11" s="3">
-        <v>1.25</v>
-      </c>
-      <c r="I11" s="37">
-        <v>0.1</v>
+        <v>0.75</v>
+      </c>
+      <c r="I11" s="26">
+        <v>0.3</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
+      <c r="A12" s="44"/>
       <c r="B12" s="15">
         <v>1.25</v>
       </c>
-      <c r="C12" s="37">
-        <v>0.2</v>
+      <c r="C12" s="26">
+        <v>0.1</v>
       </c>
       <c r="D12" s="15">
-        <v>0.75</v>
-      </c>
-      <c r="E12" s="37">
-        <v>0.1</v>
+        <v>1</v>
+      </c>
+      <c r="E12" s="26">
+        <v>0.2</v>
       </c>
       <c r="F12" s="15">
-        <v>0.75</v>
-      </c>
-      <c r="G12" s="37">
+        <v>1</v>
+      </c>
+      <c r="G12" s="26">
         <v>0.1</v>
       </c>
       <c r="H12" s="3">
-        <v>1.25</v>
-      </c>
-      <c r="I12" s="37">
+        <v>0.75</v>
+      </c>
+      <c r="I12" s="26">
         <v>0.2</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
+      <c r="A13" s="44"/>
       <c r="B13" s="15">
-        <v>0.75</v>
-      </c>
-      <c r="C13" s="37">
+        <v>1.25</v>
+      </c>
+      <c r="C13" s="26">
         <v>0.2</v>
       </c>
       <c r="D13" s="15">
-        <v>0.75</v>
-      </c>
-      <c r="E13" s="37">
-        <v>0.2</v>
+        <v>1.25</v>
+      </c>
+      <c r="E13" s="26">
+        <v>0.1</v>
       </c>
       <c r="F13" s="15">
-        <v>1.25</v>
-      </c>
-      <c r="G13" s="37">
-        <v>0.3</v>
+        <v>0.75</v>
+      </c>
+      <c r="G13" s="26">
+        <v>0.2</v>
       </c>
       <c r="H13" s="3">
         <v>0.75</v>
       </c>
-      <c r="I13" s="37">
-        <v>0.2</v>
+      <c r="I13" s="26">
+        <v>0.1</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
+      <c r="A14" s="45"/>
       <c r="B14" s="14">
         <v>0.75</v>
       </c>
@@ -2097,258 +2097,258 @@
         <v>0.1</v>
       </c>
       <c r="D14" s="14">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="E14" s="12">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="F14" s="14">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="G14" s="12">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="H14" s="4">
         <v>1</v>
       </c>
       <c r="I14" s="12">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="43" t="s">
         <v>38</v>
       </c>
       <c r="B15" s="13">
-        <v>0.75</v>
-      </c>
-      <c r="C15" s="30">
+        <v>1.25</v>
+      </c>
+      <c r="C15" s="20">
         <v>0.2</v>
       </c>
       <c r="D15" s="13">
-        <v>1.25</v>
-      </c>
-      <c r="E15" s="30">
-        <v>0.3</v>
+        <v>0.75</v>
+      </c>
+      <c r="E15" s="20">
+        <v>0.1</v>
       </c>
       <c r="F15" s="13">
-        <v>0.75</v>
-      </c>
-      <c r="G15" s="30">
+        <v>1</v>
+      </c>
+      <c r="G15" s="20">
         <v>0.1</v>
       </c>
       <c r="H15" s="7">
-        <v>1</v>
-      </c>
-      <c r="I15" s="30">
+        <v>1.25</v>
+      </c>
+      <c r="I15" s="20">
         <v>0.3</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
+      <c r="A16" s="44"/>
       <c r="B16" s="15">
         <v>1.25</v>
       </c>
-      <c r="C16" s="37">
-        <v>0.2</v>
+      <c r="C16" s="26">
+        <v>0.3</v>
       </c>
       <c r="D16" s="15">
         <v>1.25</v>
       </c>
-      <c r="E16" s="37">
-        <v>0.1</v>
+      <c r="E16" s="26">
+        <v>0.3</v>
       </c>
       <c r="F16" s="15">
         <v>1</v>
       </c>
-      <c r="G16" s="37">
+      <c r="G16" s="26">
         <v>0.2</v>
       </c>
       <c r="H16" s="3">
-        <v>0.75</v>
-      </c>
-      <c r="I16" s="37">
-        <v>0.2</v>
+        <v>1.25</v>
+      </c>
+      <c r="I16" s="26">
+        <v>0.1</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
+      <c r="A17" s="44"/>
       <c r="B17" s="15">
-        <v>0.75</v>
-      </c>
-      <c r="C17" s="37">
-        <v>0.3</v>
+        <v>1</v>
+      </c>
+      <c r="C17" s="26">
+        <v>0.2</v>
       </c>
       <c r="D17" s="15">
-        <v>1.25</v>
-      </c>
-      <c r="E17" s="37">
-        <v>0.2</v>
+        <v>1</v>
+      </c>
+      <c r="E17" s="26">
+        <v>0.3</v>
       </c>
       <c r="F17" s="15">
         <v>1.25</v>
       </c>
-      <c r="G17" s="37">
+      <c r="G17" s="26">
         <v>0.1</v>
       </c>
       <c r="H17" s="3">
-        <v>0.75</v>
-      </c>
-      <c r="I17" s="37">
-        <v>0.3</v>
+        <v>1</v>
+      </c>
+      <c r="I17" s="26">
+        <v>0.2</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
+      <c r="A18" s="44"/>
       <c r="B18" s="15">
-        <v>1</v>
-      </c>
-      <c r="C18" s="37">
-        <v>0.2</v>
+        <v>0.75</v>
+      </c>
+      <c r="C18" s="26">
+        <v>0.1</v>
       </c>
       <c r="D18" s="15">
-        <v>1</v>
-      </c>
-      <c r="E18" s="37">
-        <v>0.2</v>
+        <v>1.25</v>
+      </c>
+      <c r="E18" s="26">
+        <v>0.1</v>
       </c>
       <c r="F18" s="15">
         <v>0.75</v>
       </c>
-      <c r="G18" s="37">
+      <c r="G18" s="26">
         <v>0.2</v>
       </c>
       <c r="H18" s="3">
-        <v>1.25</v>
-      </c>
-      <c r="I18" s="37">
-        <v>0.2</v>
+        <v>0.75</v>
+      </c>
+      <c r="I18" s="26">
+        <v>0.1</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
+      <c r="A19" s="44"/>
       <c r="B19" s="15">
-        <v>0.75</v>
-      </c>
-      <c r="C19" s="37">
-        <v>0.1</v>
+        <v>1</v>
+      </c>
+      <c r="C19" s="26">
+        <v>0.3</v>
       </c>
       <c r="D19" s="15">
-        <v>1</v>
-      </c>
-      <c r="E19" s="37">
-        <v>0.1</v>
+        <v>0.75</v>
+      </c>
+      <c r="E19" s="26">
+        <v>0.2</v>
       </c>
       <c r="F19" s="15">
-        <v>1.25</v>
-      </c>
-      <c r="G19" s="37">
-        <v>0.2</v>
+        <v>0.75</v>
+      </c>
+      <c r="G19" s="26">
+        <v>0.3</v>
       </c>
       <c r="H19" s="3">
-        <v>1.25</v>
-      </c>
-      <c r="I19" s="37">
-        <v>0.3</v>
+        <v>0.75</v>
+      </c>
+      <c r="I19" s="26">
+        <v>0.2</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
+      <c r="A20" s="44"/>
       <c r="B20" s="15">
         <v>1</v>
       </c>
-      <c r="C20" s="37">
+      <c r="C20" s="26">
         <v>0.1</v>
       </c>
       <c r="D20" s="15">
-        <v>0.75</v>
-      </c>
-      <c r="E20" s="37">
-        <v>0.1</v>
+        <v>1.25</v>
+      </c>
+      <c r="E20" s="26">
+        <v>0.2</v>
       </c>
       <c r="F20" s="15">
-        <v>1</v>
-      </c>
-      <c r="G20" s="37">
+        <v>0.75</v>
+      </c>
+      <c r="G20" s="26">
         <v>0.1</v>
       </c>
       <c r="H20" s="3">
-        <v>1</v>
-      </c>
-      <c r="I20" s="37">
+        <v>1.25</v>
+      </c>
+      <c r="I20" s="26">
         <v>0.2</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
+      <c r="A21" s="44"/>
       <c r="B21" s="15">
-        <v>1.25</v>
-      </c>
-      <c r="C21" s="37">
-        <v>0.1</v>
+        <v>0.75</v>
+      </c>
+      <c r="C21" s="26">
+        <v>0.3</v>
       </c>
       <c r="D21" s="15">
         <v>0.75</v>
       </c>
-      <c r="E21" s="37">
+      <c r="E21" s="26">
         <v>0.3</v>
       </c>
       <c r="F21" s="15">
-        <v>1.25</v>
-      </c>
-      <c r="G21" s="37">
+        <v>1</v>
+      </c>
+      <c r="G21" s="26">
         <v>0.3</v>
       </c>
       <c r="H21" s="3">
         <v>1</v>
       </c>
-      <c r="I21" s="37">
-        <v>0.1</v>
+      <c r="I21" s="26">
+        <v>0.3</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="20"/>
+      <c r="A22" s="44"/>
       <c r="B22" s="15">
-        <v>1</v>
-      </c>
-      <c r="C22" s="37">
-        <v>0.3</v>
+        <v>0.75</v>
+      </c>
+      <c r="C22" s="26">
+        <v>0.2</v>
       </c>
       <c r="D22" s="15">
         <v>1</v>
       </c>
-      <c r="E22" s="37">
-        <v>0.3</v>
+      <c r="E22" s="26">
+        <v>0.1</v>
       </c>
       <c r="F22" s="15">
-        <v>0.75</v>
-      </c>
-      <c r="G22" s="37">
-        <v>0.3</v>
+        <v>1.25</v>
+      </c>
+      <c r="G22" s="26">
+        <v>0.2</v>
       </c>
       <c r="H22" s="3">
-        <v>1.25</v>
-      </c>
-      <c r="I22" s="37">
+        <v>1</v>
+      </c>
+      <c r="I22" s="26">
         <v>0.1</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
+      <c r="A23" s="45"/>
       <c r="B23" s="14">
         <v>1.25</v>
       </c>
       <c r="C23" s="12">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="D23" s="14">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="E23" s="12">
         <v>0.2</v>
       </c>
       <c r="F23" s="14">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="G23" s="12">
         <v>0.3</v>
@@ -2357,240 +2357,240 @@
         <v>0.75</v>
       </c>
       <c r="I23" s="12">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="44" t="s">
         <v>39</v>
       </c>
       <c r="B24" s="15">
-        <v>1.25</v>
-      </c>
-      <c r="C24" s="37">
+        <v>1</v>
+      </c>
+      <c r="C24" s="26">
         <v>0.1</v>
       </c>
       <c r="D24" s="15">
-        <v>1</v>
-      </c>
-      <c r="E24" s="37">
-        <v>0.2</v>
+        <v>1.25</v>
+      </c>
+      <c r="E24" s="26">
+        <v>0.1</v>
       </c>
       <c r="F24" s="15">
-        <v>1.25</v>
-      </c>
-      <c r="G24" s="37">
-        <v>0.3</v>
+        <v>1</v>
+      </c>
+      <c r="G24" s="26">
+        <v>0.1</v>
       </c>
       <c r="H24" s="3">
-        <v>0.75</v>
-      </c>
-      <c r="I24" s="37">
-        <v>0.3</v>
+        <v>1.25</v>
+      </c>
+      <c r="I24" s="26">
+        <v>0.1</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="20"/>
+      <c r="A25" s="44"/>
       <c r="B25" s="15">
-        <v>0.75</v>
-      </c>
-      <c r="C25" s="37">
-        <v>0.1</v>
+        <v>1</v>
+      </c>
+      <c r="C25" s="26">
+        <v>0.2</v>
       </c>
       <c r="D25" s="15">
-        <v>0.75</v>
-      </c>
-      <c r="E25" s="37">
-        <v>0.3</v>
+        <v>1</v>
+      </c>
+      <c r="E25" s="26">
+        <v>0.1</v>
       </c>
       <c r="F25" s="15">
-        <v>0.75</v>
-      </c>
-      <c r="G25" s="37">
-        <v>0.2</v>
+        <v>1.25</v>
+      </c>
+      <c r="G25" s="26">
+        <v>0.1</v>
       </c>
       <c r="H25" s="3">
-        <v>0.75</v>
-      </c>
-      <c r="I25" s="37">
-        <v>0.1</v>
+        <v>1.25</v>
+      </c>
+      <c r="I25" s="26">
+        <v>0.3</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="20"/>
+      <c r="A26" s="44"/>
       <c r="B26" s="15">
-        <v>1.25</v>
-      </c>
-      <c r="C26" s="37">
-        <v>0.2</v>
+        <v>1</v>
+      </c>
+      <c r="C26" s="26">
+        <v>0.3</v>
       </c>
       <c r="D26" s="15">
         <v>0.75</v>
       </c>
-      <c r="E26" s="37">
-        <v>0.2</v>
+      <c r="E26" s="26">
+        <v>0.3</v>
       </c>
       <c r="F26" s="15">
         <v>0.75</v>
       </c>
-      <c r="G26" s="37">
-        <v>0.3</v>
+      <c r="G26" s="26">
+        <v>0.2</v>
       </c>
       <c r="H26" s="3">
-        <v>0.75</v>
-      </c>
-      <c r="I26" s="37">
+        <v>1</v>
+      </c>
+      <c r="I26" s="26">
         <v>0.2</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="20"/>
+      <c r="A27" s="44"/>
       <c r="B27" s="15">
-        <v>0.75</v>
-      </c>
-      <c r="C27" s="37">
-        <v>0.3</v>
+        <v>1.25</v>
+      </c>
+      <c r="C27" s="26">
+        <v>0.2</v>
       </c>
       <c r="D27" s="15">
         <v>1.25</v>
       </c>
-      <c r="E27" s="37">
+      <c r="E27" s="26">
         <v>0.2</v>
       </c>
       <c r="F27" s="15">
-        <v>1</v>
-      </c>
-      <c r="G27" s="37">
-        <v>0.3</v>
+        <v>1.25</v>
+      </c>
+      <c r="G27" s="26">
+        <v>0.2</v>
       </c>
       <c r="H27" s="3">
-        <v>1.25</v>
-      </c>
-      <c r="I27" s="37">
-        <v>0.2</v>
+        <v>1</v>
+      </c>
+      <c r="I27" s="26">
+        <v>0.1</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="20"/>
+      <c r="A28" s="44"/>
       <c r="B28" s="15">
-        <v>1</v>
-      </c>
-      <c r="C28" s="37">
+        <v>0.75</v>
+      </c>
+      <c r="C28" s="26">
         <v>0.1</v>
       </c>
       <c r="D28" s="15">
-        <v>0.75</v>
-      </c>
-      <c r="E28" s="37">
-        <v>0.1</v>
+        <v>1</v>
+      </c>
+      <c r="E28" s="26">
+        <v>0.3</v>
       </c>
       <c r="F28" s="15">
-        <v>1</v>
-      </c>
-      <c r="G28" s="37">
-        <v>0.1</v>
+        <v>1.25</v>
+      </c>
+      <c r="G28" s="26">
+        <v>0.3</v>
       </c>
       <c r="H28" s="3">
-        <v>1.25</v>
-      </c>
-      <c r="I28" s="37">
+        <v>0.75</v>
+      </c>
+      <c r="I28" s="26">
         <v>0.3</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
+      <c r="A29" s="44"/>
       <c r="B29" s="15">
-        <v>1.25</v>
-      </c>
-      <c r="C29" s="37">
-        <v>0.3</v>
+        <v>0.75</v>
+      </c>
+      <c r="C29" s="26">
+        <v>0.2</v>
       </c>
       <c r="D29" s="15">
-        <v>1</v>
-      </c>
-      <c r="E29" s="37">
+        <v>0.75</v>
+      </c>
+      <c r="E29" s="26">
         <v>0.1</v>
       </c>
       <c r="F29" s="15">
-        <v>1.25</v>
-      </c>
-      <c r="G29" s="37">
-        <v>0.1</v>
+        <v>1</v>
+      </c>
+      <c r="G29" s="26">
+        <v>0.3</v>
       </c>
       <c r="H29" s="3">
-        <v>1</v>
-      </c>
-      <c r="I29" s="37">
-        <v>0.3</v>
+        <v>0.75</v>
+      </c>
+      <c r="I29" s="26">
+        <v>0.1</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="20"/>
+      <c r="A30" s="44"/>
       <c r="B30" s="15">
-        <v>0.75</v>
-      </c>
-      <c r="C30" s="37">
-        <v>0.2</v>
+        <v>1.25</v>
+      </c>
+      <c r="C30" s="26">
+        <v>0.1</v>
       </c>
       <c r="D30" s="15">
-        <v>1</v>
-      </c>
-      <c r="E30" s="37">
+        <v>1.25</v>
+      </c>
+      <c r="E30" s="26">
         <v>0.3</v>
       </c>
       <c r="F30" s="15">
         <v>1</v>
       </c>
-      <c r="G30" s="37">
+      <c r="G30" s="26">
         <v>0.2</v>
       </c>
       <c r="H30" s="3">
-        <v>1</v>
-      </c>
-      <c r="I30" s="37">
-        <v>0.1</v>
+        <v>1.25</v>
+      </c>
+      <c r="I30" s="26">
+        <v>0.2</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="20"/>
+      <c r="A31" s="44"/>
       <c r="B31" s="15">
-        <v>1</v>
-      </c>
-      <c r="C31" s="37">
+        <v>0.75</v>
+      </c>
+      <c r="C31" s="26">
         <v>0.3</v>
       </c>
       <c r="D31" s="15">
-        <v>1.25</v>
-      </c>
-      <c r="E31" s="37">
-        <v>0.3</v>
+        <v>0.75</v>
+      </c>
+      <c r="E31" s="26">
+        <v>0.2</v>
       </c>
       <c r="F31" s="15">
-        <v>1.25</v>
-      </c>
-      <c r="G31" s="37">
-        <v>0.2</v>
+        <v>0.75</v>
+      </c>
+      <c r="G31" s="26">
+        <v>0.3</v>
       </c>
       <c r="H31" s="3">
-        <v>1</v>
-      </c>
-      <c r="I31" s="37">
+        <v>0.75</v>
+      </c>
+      <c r="I31" s="26">
         <v>0.2</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="21"/>
+      <c r="A32" s="45"/>
       <c r="B32" s="14">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="C32" s="12">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="D32" s="14">
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="E32" s="12">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="F32" s="14">
         <v>0.75</v>
@@ -2599,22 +2599,22 @@
         <v>0.1</v>
       </c>
       <c r="H32" s="4">
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="I32" s="12">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A14"/>
     <mergeCell ref="A15:A23"/>
     <mergeCell ref="A24:A32"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>